<commit_message>
Update : Change Lembaga to Divisi Unit
</commit_message>
<xml_diff>
--- a/_Page/Anggota/Template-Anggota.xlsx
+++ b/_Page/Anggota/Template-Anggota.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\koperasi_v2\_Page\Anggota\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\koperasi_v3\_Page\Anggota\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B1DEFBC-ABFF-4A22-9843-4EAFDEF025EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF123A7-CC23-4D40-B94F-6454ED2A364B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
   <si>
     <t>No</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Kontak</t>
   </si>
   <si>
-    <t>Lembaga</t>
-  </si>
-  <si>
     <t>Ranking</t>
   </si>
   <si>
@@ -358,13 +355,46 @@
     <t>anggota20</t>
   </si>
   <si>
-    <t>Lembaga A</t>
-  </si>
-  <si>
-    <t>Lembaga B</t>
-  </si>
-  <si>
     <t>Keluar</t>
+  </si>
+  <si>
+    <t>Divisi/Unit</t>
+  </si>
+  <si>
+    <t>Divisi 1</t>
+  </si>
+  <si>
+    <t>Divisi 2</t>
+  </si>
+  <si>
+    <t>Divisi 3</t>
+  </si>
+  <si>
+    <t>Divisi 4</t>
+  </si>
+  <si>
+    <t>Divisi 5</t>
+  </si>
+  <si>
+    <t>Divisi 6</t>
+  </si>
+  <si>
+    <t>Divisi 7</t>
+  </si>
+  <si>
+    <t>Divisi 8</t>
+  </si>
+  <si>
+    <t>Divisi 9</t>
+  </si>
+  <si>
+    <t>Divisi 10</t>
+  </si>
+  <si>
+    <t>Divisi 11</t>
+  </si>
+  <si>
+    <t>Divisi 12</t>
   </si>
 </sst>
 </file>
@@ -727,7 +757,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,48 +794,48 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2">
         <v>890000001</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="4">
         <v>45304</v>
@@ -813,31 +843,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3">
         <v>890000002</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="4">
         <v>45305</v>
@@ -845,31 +875,31 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4">
         <v>890000003</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="4">
         <v>45306</v>
@@ -877,31 +907,31 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5">
         <v>890000004</v>
       </c>
       <c r="G5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J5" s="4">
         <v>45307</v>
@@ -912,31 +942,31 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6">
         <v>890000005</v>
       </c>
       <c r="G6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="4">
         <v>45308</v>
@@ -944,31 +974,31 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7">
         <v>890000006</v>
       </c>
       <c r="G7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" s="4">
         <v>45309</v>
@@ -976,31 +1006,31 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8">
         <v>890000007</v>
       </c>
       <c r="G8" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8" s="4">
         <v>45310</v>
@@ -1008,31 +1038,31 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9">
         <v>890000008</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J9" s="4">
         <v>45311</v>
@@ -1043,31 +1073,31 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F10">
         <v>890000009</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="4">
         <v>45312</v>
@@ -1075,31 +1105,31 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11">
         <v>890000010</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" s="4">
         <v>45313</v>
@@ -1107,31 +1137,31 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F12">
         <v>890000011</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" s="4">
         <v>45314</v>
@@ -1139,31 +1169,31 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13">
         <v>890000012</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" s="4">
         <v>45315</v>
@@ -1171,31 +1201,31 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14">
         <v>890000013</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14" s="4">
         <v>45316</v>
@@ -1203,31 +1233,31 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15">
         <v>890000014</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15" s="4">
         <v>45317</v>
@@ -1235,31 +1265,31 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F16">
         <v>890000015</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J16" s="4">
         <v>45318</v>
@@ -1267,31 +1297,31 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17">
         <v>890000016</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="H17">
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" s="4">
         <v>45319</v>
@@ -1299,31 +1329,31 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18">
         <v>890000017</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J18" s="4">
         <v>45320</v>
@@ -1334,31 +1364,31 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19">
         <v>890000018</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19" s="4">
         <v>45321</v>
@@ -1366,31 +1396,31 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20">
         <v>890000019</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20" s="4">
         <v>45322</v>
@@ -1398,31 +1428,31 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21">
         <v>890000020</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="4">
         <v>45323</v>

</xml_diff>